<commit_message>
?????? ??????????? ??????? ?????? ?????????? ?????????. ???????? ???????? ??????.
</commit_message>
<xml_diff>
--- a/src/tests/test_data/linux/xlsx/test-pagebreaks.xlsx
+++ b/src/tests/test_data/linux/xlsx/test-pagebreaks.xlsx
@@ -33,7 +33,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D6" authorId="0">
+    <comment ref="C3" authorId="0">
       <text>
         <r>
           <rPr>
@@ -47,29 +47,51 @@
         </r>
       </text>
     </comment>
+    <comment ref="A4" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="204"/>
+          </rPr>
+          <t>+bottom</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A7" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="204"/>
+          </rPr>
+          <t>-bottom</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
-    <t>line</t>
+    <t>Строка</t>
   </si>
   <si>
-    <t>endline</t>
+    <t>Конец строки</t>
   </si>
   <si>
-    <t>line-page</t>
+    <t>Конец подвала</t>
   </si>
   <si>
-    <t>startline</t>
-  </si>
-  <si>
-    <t>up</t>
-  </si>
-  <si>
-    <t>down</t>
+    <t>Подвал</t>
   </si>
 </sst>
 </file>
@@ -113,8 +135,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -416,10 +444,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -428,39 +456,55 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D2" t="s">
-        <v>4</v>
+      <c r="A2" s="2"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="2"/>
+      <c r="C3" s="1" t="s">
+        <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
+      <c r="D3" s="1"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="1"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="1"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>5</v>
-      </c>
-      <c r="D6" t="s">
-        <v>1</v>
-      </c>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
     </row>
   </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="A4:D4"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="A7:D7"/>
+    <mergeCell ref="A5:A6"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
   <rowBreaks count="2" manualBreakCount="2">
-    <brk id="3" max="16383" man="1"/>
-    <brk id="6" max="16383" man="1"/>
+    <brk id="5" max="16383" man="1"/>
+    <brk id="7" max="16383" man="1"/>
   </rowBreaks>
   <colBreaks count="2" manualBreakCount="2">
     <brk id="2" max="1048575" man="1"/>

</xml_diff>